<commit_message>
Saving extraction differences to data service
</commit_message>
<xml_diff>
--- a/Data/Exports/Invoice_1-1.xlsx
+++ b/Data/Exports/Invoice_1-1.xlsx
@@ -106,7 +106,7 @@
     <x:t>30 days</x:t>
   </x:si>
   <x:si>
-    <x:t>47088.46</x:t>
+    <x:t>4000</x:t>
   </x:si>
   <x:si>
     <x:t>247834.00</x:t>
@@ -171,7 +171,7 @@
     <x:t>42000.00</x:t>
   </x:si>
   <x:si>
-    <x:t>Shipboard Computer "Eddie"</x:t>
+    <x:t>Shipboard Computer</x:t>
   </x:si>
   <x:si>
     <x:t>17</x:t>

</xml_diff>

<commit_message>
Tested with Action Center - OK
</commit_message>
<xml_diff>
--- a/Data/Exports/Invoice_1-1.xlsx
+++ b/Data/Exports/Invoice_1-1.xlsx
@@ -19,28 +19,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
-    <x:t>Name</x:t>
+    <x:t>Receipt Name</x:t>
   </x:si>
   <x:si>
     <x:t>Vendor Address</x:t>
   </x:si>
   <x:si>
-    <x:t>Billing Name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Billing Address</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Billing VAT Number</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Shipping Address</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Payment Address</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vendor VAT Number</x:t>
+    <x:t>Phone Number</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Receipt Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Receipt Number</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tax Amount</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Total Value</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Items</x:t>
   </x:si>
   <x:si>
     <x:t>Date</x:t>
@@ -61,9 +61,6 @@
     <x:t>Shipping Charges</x:t>
   </x:si>
   <x:si>
-    <x:t>Tax Amount</x:t>
-  </x:si>
-  <x:si>
     <x:t>Net Amount</x:t>
   </x:si>
   <x:si>
@@ -73,33 +70,30 @@
     <x:t>Discount</x:t>
   </x:si>
   <x:si>
-    <x:t>Items</x:t>
-  </x:si>
-  <x:si>
     <x:t>Sirius Cybernetics Corp.</x:t>
   </x:si>
   <x:si>
     <x:t>4592 Bell Street New York, NY 10018</x:t>
   </x:si>
   <x:si>
-    <x:t>CHOAM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>27 Shield Wall Ave, Carthag, CH 1965 Arrakis</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CHOAM 27 Shield Wall Ave, Carthag, CH 1965 Arrakis</x:t>
-  </x:si>
-  <x:si>
     <x:t>2016-01-27</x:t>
   </x:si>
   <x:si>
+    <x:t>890127</x:t>
+  </x:si>
+  <x:si>
+    <x:t>47088.46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>294922.47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>table</x:t>
+  </x:si>
+  <x:si>
     <x:t>2016-02-26</x:t>
   </x:si>
   <x:si>
-    <x:t>890127</x:t>
-  </x:si>
-  <x:si>
     <x:t>16012633</x:t>
   </x:si>
   <x:si>
@@ -115,36 +109,7 @@
     <x:t>294922.46</x:t>
   </x:si>
   <x:si>
-    <x:t>table</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Key,Value
-"Address Line 1","4592 Bell Street"
-"City","New York"
-"Country","United States"
-"State / County / Province","New York"
-"Zip Postal Code","10018"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Key,Value
-"Address Line 1","27 Shield Ave Carthag CH Arrakis"
-"City","Wall"
-"Zip Postal Code","1965"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Key,Value
-"Address Line 1","CHOAM 27 Shield Ave Carthag CH Arrakis"
-"City","Wall"
-"Zip Postal Code","1965"</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Line Number</x:t>
-  </x:si>
-  <x:si>
     <x:t>Description</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Item PO Number</x:t>
   </x:si>
   <x:si>
     <x:t>Quantity</x:t>
@@ -606,63 +571,69 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="O1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="P1" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="P1" s="0" t="s">
+      <x:c r="Q1" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="Q1" s="0" t="s">
+      <x:c r="R1" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="R1" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
       <x:c r="S1" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:19">
       <x:c r="A2" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="F2" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="H2" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="J2" s="0" t="s">
+      <x:c r="K2" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="L2" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="K2" s="0" t="s">
+      <x:c r="M2" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="L2" s="0" t="s">
+      <x:c r="O2" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="M2" s="0" t="s">
+      <x:c r="P2" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="O2" s="0" t="s">
+      <x:c r="Q2" s="0" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="P2" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="Q2" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
       <x:c r="S2" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -729,63 +700,69 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="O1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="P1" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="P1" s="0" t="s">
+      <x:c r="Q1" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="Q1" s="0" t="s">
+      <x:c r="R1" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="R1" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
       <x:c r="S1" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:19">
       <x:c r="A2" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B2" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D2" s="1" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="B2" s="1" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F2" s="1" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="D2" s="1" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="F2" s="1" t="s">
-        <x:v>35</x:v>
+      <x:c r="G2" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>23</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="J2" s="0" t="s">
+      <x:c r="K2" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="L2" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="K2" s="0" t="s">
+      <x:c r="M2" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="L2" s="0" t="s">
+      <x:c r="O2" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="M2" s="0" t="s">
+      <x:c r="P2" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="O2" s="0" t="s">
+      <x:c r="Q2" s="0" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="P2" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="Q2" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
       <x:c r="S2" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -810,67 +787,85 @@
   <x:sheetData>
     <x:row r="1" spans="1:7">
       <x:c r="A1" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:7">
+      <x:c r="A2" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="B1" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C1" s="0" t="s">
+      <x:c r="D2" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="D1" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:7">
+      <x:c r="A3" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="E1" s="0" t="s">
+      <x:c r="B3" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="F1" s="0" t="s">
+      <x:c r="C3" s="0" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="G1" s="0" t="s">
+      <x:c r="D3" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:7">
-      <x:c r="B2" s="0" t="s">
+      <x:c r="E3" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:7">
+      <x:c r="A4" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="B4" s="0" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="C4" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="D4" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:7">
-      <x:c r="B3" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:7">
-      <x:c r="B4" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -895,67 +890,85 @@
   <x:sheetData>
     <x:row r="1" spans="1:7">
       <x:c r="A1" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:7">
+      <x:c r="A2" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C1" s="0" t="s">
+      <x:c r="D2" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="D1" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:7">
+      <x:c r="A3" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="E1" s="0" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="F1" s="0" t="s">
+      <x:c r="B3" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="G1" s="0" t="s">
+      <x:c r="D3" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:7">
-      <x:c r="B2" s="0" t="s">
+      <x:c r="E3" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:7">
+      <x:c r="A4" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="B4" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="D4" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:7">
-      <x:c r="B3" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:7">
-      <x:c r="B4" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Tested changing null values
</commit_message>
<xml_diff>
--- a/Data/Exports/Invoice_1-1.xlsx
+++ b/Data/Exports/Invoice_1-1.xlsx
@@ -19,99 +19,144 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
-    <x:t>Receipt Name</x:t>
+    <x:t>Name</x:t>
   </x:si>
   <x:si>
     <x:t>Vendor Address</x:t>
   </x:si>
   <x:si>
-    <x:t>Phone Number</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Receipt Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Receipt Number</x:t>
+    <x:t>Billing Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Billing Address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Billing VAT Number</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shipping Address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Payment Address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor VAT Number</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DueDate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Invoice Number</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PO Number</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Payment Terms</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shipping Charges</x:t>
   </x:si>
   <x:si>
     <x:t>Tax Amount</x:t>
   </x:si>
   <x:si>
-    <x:t>Total Value</x:t>
+    <x:t>Net Amount</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Total</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Discount</x:t>
   </x:si>
   <x:si>
     <x:t>Items</x:t>
   </x:si>
   <x:si>
-    <x:t>Date</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DueDate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Invoice Number</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PO Number</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Payment Terms</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Shipping Charges</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Net Amount</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Total</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Discount</x:t>
-  </x:si>
-  <x:si>
     <x:t>Sirius Cybernetics Corp.</x:t>
   </x:si>
   <x:si>
     <x:t>4592 Bell Street New York, NY 10018</x:t>
   </x:si>
   <x:si>
+    <x:t>CHOAM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27 Shield Wall Ave, Carthag, CH 1965 Arrakis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CHOAM 27 Shield Wall Ave, Carthag, CH 1965 Arrakis</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bill To</x:t>
+  </x:si>
+  <x:si>
     <x:t>2016-01-27</x:t>
   </x:si>
   <x:si>
+    <x:t>2016-02-26</x:t>
+  </x:si>
+  <x:si>
     <x:t>890127</x:t>
   </x:si>
   <x:si>
+    <x:t>30 days</x:t>
+  </x:si>
+  <x:si>
     <x:t>47088.46</x:t>
   </x:si>
   <x:si>
-    <x:t>294922.47</x:t>
+    <x:t>247834.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>294922.46</x:t>
   </x:si>
   <x:si>
     <x:t>table</x:t>
   </x:si>
   <x:si>
-    <x:t>2016-02-26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16012633</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30 days</x:t>
-  </x:si>
-  <x:si>
-    <x:t>40000</x:t>
-  </x:si>
-  <x:si>
-    <x:t>247834.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>294922.46</x:t>
+    <x:t>Key,Value
+"Address Line 1","4592 Bell Street"
+"City","New York"
+"Country","United States"
+"State / County / Province","New York"
+"Zip Postal Code","10018"</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Key,Value
+"Address Line 1","27 Shield Ave Carthag CH Arrakis"
+"City","Wall"
+"Zip Postal Code","1965"</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Key,Value
+"Address Line 1","CHOAM 27 Shield Ave Carthag CH Arrakis"
+"City","Wall"
+"Zip Postal Code","1965"</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Key,Value
+"Address Line 1","To"
+"Address Line 2",""
+"Address Line 3",""
+"City","Bill"
+"Country","United States"
+"State / County / Province","Wyoming"
+"Zip Postal Code",""</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Line Number</x:t>
   </x:si>
   <x:si>
     <x:t>Description</x:t>
   </x:si>
   <x:si>
+    <x:t>Item PO Number</x:t>
+  </x:si>
+  <x:si>
     <x:t>Quantity</x:t>
   </x:si>
   <x:si>
@@ -136,7 +181,7 @@
     <x:t>42000.00</x:t>
   </x:si>
   <x:si>
-    <x:t>Shipboard Computer</x:t>
+    <x:t>Shipboard Computer "Eddie"</x:t>
   </x:si>
   <x:si>
     <x:t>17</x:t>
@@ -571,69 +616,63 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="O1" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="P1" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="Q1" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="R1" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="S1" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:19">
       <x:c r="A2" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G2" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="J2" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="K2" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="L2" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="M2" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="O2" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="P2" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="Q2" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="S2" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -700,69 +739,63 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="O1" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="P1" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="Q1" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="R1" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="S1" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:19">
       <x:c r="A2" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B2" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D2" s="1" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F2" s="1" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G2" s="1" t="s">
+        <x:v>36</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="J2" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="K2" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="L2" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="M2" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="O2" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="P2" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="Q2" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="S2" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -787,85 +820,67 @@
   <x:sheetData>
     <x:row r="1" spans="1:7">
       <x:c r="A1" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F1" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G1" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:7">
-      <x:c r="A2" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:7">
-      <x:c r="A3" s="0" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>40</x:v>
-      </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
-      <x:c r="A4" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -890,85 +905,67 @@
   <x:sheetData>
     <x:row r="1" spans="1:7">
       <x:c r="A1" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="F1" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G1" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:7">
-      <x:c r="A2" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
       <x:c r="B2" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
     </x:row>
     <x:row r="3" spans="1:7">
-      <x:c r="A3" s="0" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
+      <x:c r="C3" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
-      <x:c r="A4" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>55</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>